<commit_message>
Chrome and firefox issue sorted
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/TestData.xlsx
+++ b/src/main/resources/testData/TestData.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SUSUniversity\SRSUniversity\src\main\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SRSUniversity\SRSUniversity\src\main\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1A96A9-DC94-4EDF-A0AA-EF6FD37C6A61}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginData" sheetId="1" r:id="rId1"/>
     <sheet name="InvalidUserNameLogin" sheetId="2" r:id="rId2"/>
-    <sheet name="InvalidPasswordLogin" sheetId="3" r:id="rId3"/>
+    <sheet name="LoginPageUI" sheetId="5" r:id="rId3"/>
+    <sheet name="InvalidPasswordLogin" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>UserName</t>
   </si>
@@ -61,11 +63,26 @@
   <si>
     <t>Ci Anywhere Workplace</t>
   </si>
+  <si>
+    <t>Log on using your details</t>
+  </si>
+  <si>
+    <t>View Terms and Conditions</t>
+  </si>
+  <si>
+    <t>loginpagetitle</t>
+  </si>
+  <si>
+    <t>headerlogonmetext</t>
+  </si>
+  <si>
+    <t>verifytermsandconditions</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -394,24 +411,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="17.42578125" style="1" customWidth="1"/>
-    <col min="5" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="9.140625" style="2"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="33.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="17.44140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="9.109375" style="1"/>
+    <col min="7" max="7" width="9.109375" style="2"/>
+    <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -425,7 +442,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -446,16 +463,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,7 +483,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1011002</v>
       </c>
@@ -483,16 +500,58 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7D6AB8B-F63E-4D04-A6AD-0FC227BF3EB0}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1011002</v>
       </c>

</xml_diff>